<commit_message>
changed object for where to buy tc
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/ProductDetailsPage.xlsx
+++ b/src/test/java/com/born/xls/ProductDetailsPage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6590" windowHeight="2660" tabRatio="937" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6590" windowHeight="2660" tabRatio="937" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="159">
   <si>
     <t>TCID</t>
   </si>
@@ -602,6 +602,9 @@
       </rPr>
       <t xml:space="preserve"> button is working to add the products</t>
     </r>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1162,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,7 +1192,7 @@
         <v>157</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1200,7 +1203,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1211,7 +1214,7 @@
         <v>134</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1222,7 +1225,7 @@
         <v>135</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1233,7 +1236,7 @@
         <v>113</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1244,7 +1247,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1255,7 +1258,7 @@
         <v>116</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1266,7 +1269,7 @@
         <v>132</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1290,10 +1293,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J637"/>
+  <dimension ref="A1:K637"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1305,9 +1308,9 @@
     <col min="5" max="5" width="34.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="29.7265625" style="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.1796875" style="1" collapsed="1"/>
-    <col min="9" max="10" width="9.1796875" style="1"/>
-    <col min="11" max="16384" width="9.1796875" style="1" collapsed="1"/>
+    <col min="8" max="10" width="9.1796875" style="1" collapsed="1"/>
+    <col min="11" max="11" width="9.1796875" style="1"/>
+    <col min="12" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -8164,7 +8167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed where to buy tc steps
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/ProductDetailsPage.xlsx
+++ b/src/test/java/com/born/xls/ProductDetailsPage.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Test Steps" sheetId="3" r:id="rId2"/>
     <sheet name="PDP-Write a Review" sheetId="57" r:id="rId3"/>
     <sheet name="Comparing the Products" sheetId="58" r:id="rId4"/>
+    <sheet name="WhereToBuy" sheetId="59" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$C$8</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="162">
   <si>
     <t>TCID</t>
   </si>
@@ -394,9 +395,6 @@
   </si>
   <si>
     <t>ServicePartsPage_Link</t>
-  </si>
-  <si>
-    <t>Shop Online Where to Buy(WTB)</t>
   </si>
   <si>
     <t>Verify that 1) Contact us 2) Find a Part 3) Get Support should be there</t>
@@ -606,12 +604,25 @@
   <si>
     <t>N</t>
   </si>
+  <si>
+    <t>Result1</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>WhereToBuy</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,7 +682,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -706,6 +717,11 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -773,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -849,6 +865,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1162,15 +1179,15 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.90625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="57" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.54296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.1796875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="35.90625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="57.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="9.54296875" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1189,10 +1206,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1203,7 +1220,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1211,10 +1228,10 @@
         <v>56</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1222,10 +1239,10 @@
         <v>75</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1236,7 +1253,7 @@
         <v>113</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1247,7 +1264,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1258,7 +1275,7 @@
         <v>116</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1266,18 +1283,18 @@
         <v>115</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>62</v>
@@ -1293,27 +1310,26 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K637"/>
+  <dimension ref="A1:H637"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H102" sqref="H102"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.6328125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.1796875" style="1" collapsed="1"/>
-    <col min="3" max="3" width="54.08984375" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.7265625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="9.1796875" style="1" collapsed="1"/>
-    <col min="11" max="11" width="9.1796875" style="1"/>
-    <col min="12" max="16384" width="9.1796875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="32.6328125" collapsed="true"/>
+    <col min="2" max="2" style="1" width="9.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="54.08984375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="22.81640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="34.1796875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="29.7265625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="7.51171875" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1335,8 +1351,11 @@
       <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
@@ -1355,7 +1374,7 @@
       </c>
       <c r="G2" s="24"/>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>38</v>
       </c>
@@ -1374,7 +1393,7 @@
       </c>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
@@ -1393,7 +1412,7 @@
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -1412,7 +1431,7 @@
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
@@ -1431,7 +1450,7 @@
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>38</v>
       </c>
@@ -1450,7 +1469,7 @@
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
@@ -1469,7 +1488,7 @@
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
     </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
@@ -1486,7 +1505,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -1495,7 +1514,7 @@
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>49</v>
       </c>
@@ -1514,7 +1533,7 @@
       </c>
       <c r="G11" s="24"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
@@ -1533,7 +1552,7 @@
       </c>
       <c r="G12" s="24"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -1552,7 +1571,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1571,7 +1590,7 @@
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
@@ -1590,7 +1609,7 @@
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
@@ -1620,7 +1639,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>47</v>
@@ -1778,13 +1797,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
@@ -1797,10 +1816,10 @@
         <v>23</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
@@ -1817,10 +1836,10 @@
         <v>87</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
@@ -1836,7 +1855,7 @@
         <v>88</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>59</v>
@@ -1855,10 +1874,10 @@
         <v>87</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
@@ -1893,7 +1912,7 @@
         <v>87</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>82</v>
@@ -1949,13 +1968,13 @@
         <v>15</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
@@ -1968,10 +1987,10 @@
         <v>16</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
@@ -1988,10 +2007,10 @@
         <v>87</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
@@ -2007,7 +2026,7 @@
         <v>88</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E38" s="24" t="s">
         <v>59</v>
@@ -2026,10 +2045,10 @@
         <v>87</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="24"/>
@@ -2058,7 +2077,7 @@
         <v>56</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>89</v>
@@ -2077,7 +2096,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>58</v>
@@ -2096,7 +2115,7 @@
         <v>56</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>34</v>
@@ -2223,10 +2242,10 @@
         <v>78</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="24"/>
@@ -2261,10 +2280,10 @@
         <v>78</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F52" s="24"/>
       <c r="G52" s="24"/>
@@ -2439,10 +2458,10 @@
         <v>63</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F62" s="32"/>
       <c r="G62" s="32"/>
@@ -2578,7 +2597,7 @@
         <v>25</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D70" s="24" t="s">
         <v>11</v>
@@ -2587,7 +2606,7 @@
         <v>59</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G70" s="24"/>
     </row>
@@ -2599,13 +2618,13 @@
         <v>24</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E71" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F71" s="24"/>
       <c r="G71" s="24"/>
@@ -2618,10 +2637,10 @@
         <v>23</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D72" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E72" s="24"/>
       <c r="F72" s="24"/>
@@ -2635,13 +2654,13 @@
         <v>22</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D73" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E73" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F73" s="24"/>
       <c r="G73" s="24"/>
@@ -2654,10 +2673,10 @@
         <v>21</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E74" s="24" t="s">
         <v>59</v>
@@ -2676,7 +2695,7 @@
         <v>63</v>
       </c>
       <c r="D75" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E75" s="24" t="s">
         <v>97</v>
@@ -2714,7 +2733,7 @@
         <v>78</v>
       </c>
       <c r="D77" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E77" s="26" t="s">
         <v>104</v>
@@ -2813,7 +2832,7 @@
         <v>71</v>
       </c>
       <c r="D82" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E82" s="26" t="s">
         <v>102</v>
@@ -2848,13 +2867,13 @@
         <v>74</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D84" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="24"/>
@@ -2867,7 +2886,7 @@
         <v>96</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D85" s="24" t="s">
         <v>33</v>
@@ -2883,7 +2902,7 @@
         <v>64</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C86" s="24" t="s">
         <v>73</v>
@@ -2902,7 +2921,7 @@
         <v>64</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C87" s="24" t="s">
         <v>34</v>
@@ -3029,7 +3048,7 @@
         <v>78</v>
       </c>
       <c r="D94" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E94" s="24" t="s">
         <v>46</v>
@@ -3075,7 +3094,7 @@
       <c r="F96" s="24"/>
       <c r="G96" s="24"/>
     </row>
-    <row r="97" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="19" t="s">
         <v>114</v>
       </c>
@@ -3092,7 +3111,7 @@
       <c r="F97" s="24"/>
       <c r="G97" s="24"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="25"/>
       <c r="B98" s="25"/>
       <c r="C98" s="25"/>
@@ -3101,7 +3120,7 @@
       <c r="F98" s="25"/>
       <c r="G98" s="25"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="19" t="s">
         <v>115</v>
       </c>
@@ -3120,7 +3139,7 @@
       </c>
       <c r="G99" s="24"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="19" t="s">
         <v>115</v>
       </c>
@@ -3139,7 +3158,7 @@
       </c>
       <c r="G100" s="24"/>
     </row>
-    <row r="101" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="19" t="s">
         <v>115</v>
       </c>
@@ -3158,7 +3177,7 @@
       <c r="F101" s="24"/>
       <c r="G101" s="24"/>
     </row>
-    <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="19" t="s">
         <v>115</v>
       </c>
@@ -3166,18 +3185,18 @@
         <v>24</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D102" s="24" t="s">
         <v>32</v>
       </c>
       <c r="E102" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F102" s="24"/>
       <c r="G102" s="24"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="19" t="s">
         <v>115</v>
       </c>
@@ -3194,7 +3213,7 @@
       <c r="F103" s="24"/>
       <c r="G103" s="24"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="25"/>
       <c r="B104" s="25"/>
       <c r="C104" s="25"/>
@@ -3205,9 +3224,9 @@
       <c r="F104" s="25"/>
       <c r="G104" s="25"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B105" s="24" t="s">
         <v>27</v>
@@ -3223,10 +3242,13 @@
         <v>8</v>
       </c>
       <c r="G105" s="24"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H105" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B106" s="24" t="s">
         <v>26</v>
@@ -3242,105 +3264,123 @@
         <v>10</v>
       </c>
       <c r="G106" s="24"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H106" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B107" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C107" s="24" t="s">
-        <v>39</v>
+        <v>146</v>
       </c>
       <c r="D107" s="24" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E107" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="F107" s="24"/>
+        <v>59</v>
+      </c>
+      <c r="F107" s="24" t="s">
+        <v>60</v>
+      </c>
       <c r="G107" s="24"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H107" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B108" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C108" s="24" t="s">
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="D108" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E108" s="24" t="s">
-        <v>44</v>
+        <v>140</v>
+      </c>
+      <c r="E108" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="F108" s="24"/>
       <c r="G108" s="24"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H108" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B109" s="24" t="s">
         <v>23</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="D109" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E109" s="24" t="s">
-        <v>42</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="E109" s="24"/>
       <c r="F109" s="24"/>
       <c r="G109" s="24"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H109" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B110" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C110" s="24" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="D110" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E110" s="26" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F110" s="24"/>
       <c r="G110" s="24"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H110" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B111" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C111" s="24" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="D111" s="24" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="E111" s="24" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F111" s="24"/>
       <c r="G111" s="24"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H111" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B112" s="24" t="s">
         <v>20</v>
@@ -3349,36 +3389,42 @@
         <v>63</v>
       </c>
       <c r="D112" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E112" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F112" s="24"/>
       <c r="G112" s="24"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H112" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B113" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C113" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D113" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E113" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F113" s="24"/>
       <c r="G113" s="24"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H113" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B114" s="24" t="s">
         <v>12</v>
@@ -3387,36 +3433,42 @@
         <v>87</v>
       </c>
       <c r="D114" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E114" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F114" s="24"/>
       <c r="G114" s="24"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H114" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B115" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D115" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E115" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F115" s="24"/>
       <c r="G115" s="24"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H115" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B116" s="24" t="s">
         <v>14</v>
@@ -3425,36 +3477,42 @@
         <v>87</v>
       </c>
       <c r="D116" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E116" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F116" s="24"/>
       <c r="G116" s="24"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H116" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B117" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D117" s="24" t="s">
         <v>32</v>
       </c>
       <c r="E117" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F117" s="24"/>
       <c r="G117" s="24"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H117" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="23" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B118" s="24" t="s">
         <v>16</v>
@@ -3468,8 +3526,11 @@
       <c r="E118" s="24"/>
       <c r="F118" s="24"/>
       <c r="G118" s="24"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H118" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="10"/>
       <c r="B119" s="10"/>
       <c r="C119" s="10"/>
@@ -3478,7 +3539,7 @@
       <c r="F119" s="10"/>
       <c r="G119" s="10"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="10"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
@@ -3487,7 +3548,7 @@
       <c r="F120" s="10"/>
       <c r="G120" s="10"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="28"/>
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
@@ -3496,7 +3557,7 @@
       <c r="F121" s="10"/>
       <c r="G121" s="10"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="10"/>
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
@@ -3505,7 +3566,7 @@
       <c r="F122" s="10"/>
       <c r="G122" s="10"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="10"/>
       <c r="B123" s="10"/>
       <c r="C123" s="10"/>
@@ -3514,7 +3575,7 @@
       <c r="F123" s="10"/>
       <c r="G123" s="10"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="10"/>
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
@@ -3523,7 +3584,7 @@
       <c r="F124" s="10"/>
       <c r="G124" s="10"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="10"/>
       <c r="B125" s="10"/>
       <c r="C125" s="10"/>
@@ -3532,7 +3593,7 @@
       <c r="F125" s="10"/>
       <c r="G125" s="10"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="10"/>
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
@@ -3541,7 +3602,7 @@
       <c r="F126" s="10"/>
       <c r="G126" s="10"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="10"/>
       <c r="B127" s="10"/>
       <c r="C127" s="10"/>
@@ -3550,7 +3611,7 @@
       <c r="F127" s="10"/>
       <c r="G127" s="10"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="10"/>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
@@ -8125,13 +8186,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="36.08984375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.08984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>107</v>
@@ -8168,13 +8229,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.08984375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.08984375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.08984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -8203,4 +8264,38 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="13.453125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Marked all Tc to Yes
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/ProductDetailsPage.xlsx
+++ b/src/test/java/com/born/xls/ProductDetailsPage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="158">
   <si>
     <t>TCID</t>
   </si>
@@ -602,27 +602,14 @@
     </r>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Result1</t>
-  </si>
-  <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>WhereToBuy</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,7 +669,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -717,11 +704,6 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -789,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -865,7 +847,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,15 +1160,15 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="35.90625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="57.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="9.54296875" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="35.90625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="57" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.54296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1209,7 +1190,7 @@
         <v>156</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1220,7 +1201,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1231,7 +1212,7 @@
         <v>133</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1242,7 +1223,7 @@
         <v>134</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1253,7 +1234,7 @@
         <v>113</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1264,7 +1245,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1275,7 +1256,7 @@
         <v>116</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1286,12 +1267,12 @@
         <v>131</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>132</v>
@@ -1312,24 +1293,24 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H637"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="32.6328125" collapsed="true"/>
-    <col min="2" max="2" style="1" width="9.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="54.08984375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="22.81640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="34.1796875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="29.7265625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="7.51171875" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="32.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.1796875" style="1" collapsed="1"/>
+    <col min="3" max="3" width="54.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.1796875" style="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1351,11 +1332,8 @@
       <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="33" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
@@ -1374,7 +1352,7 @@
       </c>
       <c r="G2" s="24"/>
     </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>38</v>
       </c>
@@ -1393,7 +1371,7 @@
       </c>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
@@ -1412,7 +1390,7 @@
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -1431,7 +1409,7 @@
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
     </row>
-    <row r="6" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
@@ -1450,7 +1428,7 @@
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>38</v>
       </c>
@@ -1469,7 +1447,7 @@
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
@@ -1488,7 +1466,7 @@
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
     </row>
-    <row r="9" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
@@ -1505,7 +1483,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -1514,7 +1492,7 @@
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>49</v>
       </c>
@@ -1533,7 +1511,7 @@
       </c>
       <c r="G11" s="24"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
@@ -1552,7 +1530,7 @@
       </c>
       <c r="G12" s="24"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -1571,7 +1549,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1590,7 +1568,7 @@
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
@@ -1609,7 +1587,7 @@
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
@@ -3094,7 +3072,7 @@
       <c r="F96" s="24"/>
       <c r="G96" s="24"/>
     </row>
-    <row r="97" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="19" t="s">
         <v>114</v>
       </c>
@@ -3111,7 +3089,7 @@
       <c r="F97" s="24"/>
       <c r="G97" s="24"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="25"/>
       <c r="B98" s="25"/>
       <c r="C98" s="25"/>
@@ -3120,7 +3098,7 @@
       <c r="F98" s="25"/>
       <c r="G98" s="25"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="19" t="s">
         <v>115</v>
       </c>
@@ -3139,7 +3117,7 @@
       </c>
       <c r="G99" s="24"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="19" t="s">
         <v>115</v>
       </c>
@@ -3158,7 +3136,7 @@
       </c>
       <c r="G100" s="24"/>
     </row>
-    <row r="101" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="19" t="s">
         <v>115</v>
       </c>
@@ -3177,7 +3155,7 @@
       <c r="F101" s="24"/>
       <c r="G101" s="24"/>
     </row>
-    <row r="102" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="19" t="s">
         <v>115</v>
       </c>
@@ -3196,7 +3174,7 @@
       <c r="F102" s="24"/>
       <c r="G102" s="24"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="19" t="s">
         <v>115</v>
       </c>
@@ -3213,7 +3191,7 @@
       <c r="F103" s="24"/>
       <c r="G103" s="24"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="25"/>
       <c r="B104" s="25"/>
       <c r="C104" s="25"/>
@@ -3224,9 +3202,9 @@
       <c r="F104" s="25"/>
       <c r="G104" s="25"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B105" s="24" t="s">
         <v>27</v>
@@ -3242,13 +3220,10 @@
         <v>8</v>
       </c>
       <c r="G105" s="24"/>
-      <c r="H105" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B106" s="24" t="s">
         <v>26</v>
@@ -3264,13 +3239,10 @@
         <v>10</v>
       </c>
       <c r="G106" s="24"/>
-      <c r="H106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B107" s="24" t="s">
         <v>25</v>
@@ -3288,13 +3260,10 @@
         <v>60</v>
       </c>
       <c r="G107" s="24"/>
-      <c r="H107" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B108" s="24" t="s">
         <v>24</v>
@@ -3310,13 +3279,10 @@
       </c>
       <c r="F108" s="24"/>
       <c r="G108" s="24"/>
-      <c r="H108" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B109" s="24" t="s">
         <v>23</v>
@@ -3330,13 +3296,10 @@
       <c r="E109" s="24"/>
       <c r="F109" s="24"/>
       <c r="G109" s="24"/>
-      <c r="H109" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B110" s="24" t="s">
         <v>22</v>
@@ -3352,13 +3315,10 @@
       </c>
       <c r="F110" s="24"/>
       <c r="G110" s="24"/>
-      <c r="H110" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B111" s="24" t="s">
         <v>21</v>
@@ -3374,13 +3334,10 @@
       </c>
       <c r="F111" s="24"/>
       <c r="G111" s="24"/>
-      <c r="H111" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B112" s="24" t="s">
         <v>20</v>
@@ -3396,13 +3353,10 @@
       </c>
       <c r="F112" s="24"/>
       <c r="G112" s="24"/>
-      <c r="H112" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B113" s="24" t="s">
         <v>19</v>
@@ -3418,13 +3372,10 @@
       </c>
       <c r="F113" s="24"/>
       <c r="G113" s="24"/>
-      <c r="H113" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B114" s="24" t="s">
         <v>12</v>
@@ -3440,13 +3391,10 @@
       </c>
       <c r="F114" s="24"/>
       <c r="G114" s="24"/>
-      <c r="H114" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B115" s="24" t="s">
         <v>13</v>
@@ -3462,13 +3410,10 @@
       </c>
       <c r="F115" s="24"/>
       <c r="G115" s="24"/>
-      <c r="H115" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B116" s="24" t="s">
         <v>14</v>
@@ -3484,13 +3429,10 @@
       </c>
       <c r="F116" s="24"/>
       <c r="G116" s="24"/>
-      <c r="H116" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B117" s="24" t="s">
         <v>15</v>
@@ -3506,13 +3448,10 @@
       </c>
       <c r="F117" s="24"/>
       <c r="G117" s="24"/>
-      <c r="H117" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B118" s="24" t="s">
         <v>16</v>
@@ -3526,11 +3465,8 @@
       <c r="E118" s="24"/>
       <c r="F118" s="24"/>
       <c r="G118" s="24"/>
-      <c r="H118" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="10"/>
       <c r="B119" s="10"/>
       <c r="C119" s="10"/>
@@ -3539,7 +3475,7 @@
       <c r="F119" s="10"/>
       <c r="G119" s="10"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="10"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
@@ -3548,7 +3484,7 @@
       <c r="F120" s="10"/>
       <c r="G120" s="10"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="28"/>
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
@@ -3557,7 +3493,7 @@
       <c r="F121" s="10"/>
       <c r="G121" s="10"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="10"/>
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
@@ -3566,7 +3502,7 @@
       <c r="F122" s="10"/>
       <c r="G122" s="10"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" s="10"/>
       <c r="B123" s="10"/>
       <c r="C123" s="10"/>
@@ -3575,7 +3511,7 @@
       <c r="F123" s="10"/>
       <c r="G123" s="10"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="10"/>
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
@@ -3584,7 +3520,7 @@
       <c r="F124" s="10"/>
       <c r="G124" s="10"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="10"/>
       <c r="B125" s="10"/>
       <c r="C125" s="10"/>
@@ -3593,7 +3529,7 @@
       <c r="F125" s="10"/>
       <c r="G125" s="10"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" s="10"/>
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
@@ -3602,7 +3538,7 @@
       <c r="F126" s="10"/>
       <c r="G126" s="10"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="10"/>
       <c r="B127" s="10"/>
       <c r="C127" s="10"/>
@@ -3611,7 +3547,7 @@
       <c r="F127" s="10"/>
       <c r="G127" s="10"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="10"/>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
@@ -8186,8 +8122,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="36.08984375" collapsed="true"/>
+    <col min="1" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -8234,8 +8170,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.08984375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="1" max="1" width="16.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -8276,7 +8212,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="1" max="1" width="13.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added Test Data for failed TC
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/ProductDetailsPage.xlsx
+++ b/src/test/java/com/born/xls/ProductDetailsPage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6590" windowHeight="2660" tabRatio="937" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6590" windowHeight="2660" tabRatio="937" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -1509,10 +1509,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I637"/>
+  <dimension ref="A1:H637"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1524,9 +1524,8 @@
     <col min="5" max="5" width="34.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="29.7265625" style="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.1796875" style="1" collapsed="1"/>
-    <col min="9" max="9" width="9.1796875" style="1"/>
-    <col min="10" max="16384" width="9.1796875" style="1" collapsed="1"/>
+    <col min="8" max="8" width="9.1796875" style="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -8717,7 +8716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed keyword to Failed TC
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/ProductDetailsPage.xlsx
+++ b/src/test/java/com/born/xls/ProductDetailsPage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6590" windowHeight="2660" tabRatio="937"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6590" windowHeight="2660" tabRatio="937" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="215">
   <si>
     <t>TCID</t>
   </si>
@@ -772,6 +772,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>ClickEnter</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1372,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="105" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1512,10 +1515,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H637"/>
+  <dimension ref="A1:I637"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="D101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1527,8 +1530,9 @@
     <col min="5" max="5" width="34.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="29.7265625" style="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.1796875" style="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1" collapsed="1"/>
+    <col min="8" max="8" width="9.1796875" style="1" collapsed="1"/>
+    <col min="9" max="9" width="9.1796875" style="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -3548,7 +3552,7 @@
         <v>152</v>
       </c>
       <c r="D111" s="24" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="E111" s="24" t="s">
         <v>59</v>
@@ -8720,7 +8724,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
changed the keyword from Clickenter to enter for "Where To Buy" TC
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/ProductDetailsPage.xlsx
+++ b/src/test/java/com/born/xls/ProductDetailsPage.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="215">
   <si>
     <t>TCID</t>
   </si>
@@ -768,9 +768,6 @@
   </si>
   <si>
     <t>col|CountryName</t>
-  </si>
-  <si>
-    <t>ClickEnter</t>
   </si>
   <si>
     <t>mouseHover1</t>
@@ -1375,7 +1372,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,7 +1440,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>112</v>
@@ -1519,8 +1516,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J639"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,7 +1762,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>11</v>
@@ -2559,7 +2556,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B57" s="24" t="s">
         <v>27</v>
@@ -2578,7 +2575,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B58" s="24" t="s">
         <v>26</v>
@@ -2597,13 +2594,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B59" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>11</v>
@@ -2618,7 +2615,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B60" s="24" t="s">
         <v>24</v>
@@ -2637,7 +2634,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B61" s="24" t="s">
         <v>23</v>
@@ -2654,7 +2651,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B62" s="24" t="s">
         <v>22</v>
@@ -2673,7 +2670,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B63" s="24" t="s">
         <v>21</v>
@@ -2692,7 +2689,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B64" s="24" t="s">
         <v>20</v>
@@ -2711,7 +2708,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B65" s="24" t="s">
         <v>19</v>
@@ -2730,7 +2727,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B66" s="24" t="s">
         <v>12</v>
@@ -2749,7 +2746,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B67" s="24" t="s">
         <v>13</v>
@@ -2768,7 +2765,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B68" s="24" t="s">
         <v>14</v>
@@ -3308,7 +3305,7 @@
         <v>116</v>
       </c>
       <c r="D97" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E97" s="24" t="s">
         <v>46</v>
@@ -3590,7 +3587,7 @@
         <v>151</v>
       </c>
       <c r="D113" s="24" t="s">
-        <v>212</v>
+        <v>147</v>
       </c>
       <c r="E113" s="24" t="s">
         <v>59</v>

</xml_diff>